<commit_message>
data is now in a more usable structure, have zombie trees and specifically ones that have died and come back to life 2 or more times
</commit_message>
<xml_diff>
--- a/data/zombie_total.xlsx
+++ b/data/zombie_total.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{613B0A42-D224-4CD8-AA77-655145B95118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6168" yWindow="1980" windowWidth="17280" windowHeight="8880" xr2:uid="{B2FBE2F6-2FF5-4749-960D-0B0EF899CE93}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B2FBE2F6-2FF5-4749-960D-0B0EF899CE93}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -413,7 +413,7 @@
   <dimension ref="A1:K101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>